<commit_message>
test contact us completed
</commit_message>
<xml_diff>
--- a/com.luma/src/test/resources/test_data.xlsx
+++ b/com.luma/src/test/resources/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.luma\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0CF0EE-E9D7-463A-B571-CE2CD0AE43FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B92B64-834C-4BBB-9453-9850BE5ED1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="testDoSearch" sheetId="1" r:id="rId1"/>
     <sheet name="doSignIn" sheetId="2" r:id="rId2"/>
-    <sheet name="DoInvalidLogin" sheetId="3" r:id="rId3"/>
+    <sheet name="createAccount" sheetId="4" r:id="rId3"/>
+    <sheet name="DoInvalidLogin" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>searchterm</t>
   </si>
@@ -105,13 +106,34 @@
   </si>
   <si>
     <t>roni_cost3@example.com</t>
+  </si>
+  <si>
+    <t>abctestemail2378!!!!@gmail.com</t>
+  </si>
+  <si>
+    <t>QqwertyQ@123!</t>
+  </si>
+  <si>
+    <t>abctestemail2379!!!!@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abctestemail2370!!!!@gmail.com </t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +167,11 @@
       <name val="Open Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -175,6 +202,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -564,15 +592,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7556C8-E700-48CB-9BE6-823B0EE36C2B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -600,17 +628,75 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{C1C2F231-23E3-4826-A787-72ECC0FCC383}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{967F2E60-B855-47CF-A8B0-F697DD123EA5}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{833B8128-6393-43B6-9699-9181B4B2F039}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D45730-030E-40CA-907D-93AFB77B716D}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEB009D-A5FA-4CA7-B6A8-5006B2678784}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
tests completed and documented
</commit_message>
<xml_diff>
--- a/com.luma/src/test/resources/test_data.xlsx
+++ b/com.luma/src/test/resources/test_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.luma\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B92B64-834C-4BBB-9453-9850BE5ED1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CE436E-ADB4-4B6A-87B8-E83003EC6841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
+    <workbookView xWindow="1608" yWindow="1332" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="4" xr2:uid="{63BAD3BA-E091-40CE-9B8C-FA220E697B2E}"/>
   </bookViews>
   <sheets>
     <sheet name="testDoSearch" sheetId="1" r:id="rId1"/>
     <sheet name="doSignIn" sheetId="2" r:id="rId2"/>
     <sheet name="createAccount" sheetId="4" r:id="rId3"/>
     <sheet name="DoInvalidLogin" sheetId="3" r:id="rId4"/>
+    <sheet name="doSubscribe" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>searchterm</t>
   </si>
@@ -127,6 +128,33 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>abctestemail10@gmail.com</t>
+  </si>
+  <si>
+    <t>abctestemail20@gmail.com</t>
+  </si>
+  <si>
+    <t>abctestemail30@gmail.com</t>
+  </si>
+  <si>
+    <t>Larry</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>Amare</t>
+  </si>
+  <si>
+    <t>Dawson</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>smith</t>
   </si>
 </sst>
 </file>
@@ -665,16 +693,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D45730-030E-40CA-907D-93AFB77B716D}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -691,7 +721,54 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{89AA9D9C-0869-4ED4-B6A5-2F947D9A705A}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{BCC5A9E2-EE9F-4583-81D2-DB86E39DFDF7}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{FD18D400-9421-4BBB-A387-4677ED3F584D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -745,4 +822,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFB91B4-F41C-46C2-A076-D533810F4FFD}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{59A72CE4-8546-4898-BA56-7773E60E44D6}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{7A05E63A-A087-42C3-B1A4-14A4C0A8E4D4}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{513BBBF3-13A2-4FBA-AE42-616D07EEF364}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>